<commit_message>
update templates and admin panel and services
</commit_message>
<xml_diff>
--- a/media/export.xlsx
+++ b/media/export.xlsx
@@ -486,95 +486,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ВСОШ</t>
+          <t>ВСОШ по физре</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Журавлёв Дмитрий Сергеевич</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ппаап</t>
+          <t>Безруков Владислав Александрович</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>История</t>
+          <t>Технология</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1в</t>
+          <t>9в</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Исскуство</t>
+          <t>Спорт</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Городской</t>
+          <t>Школьный</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Лауреат</t>
+          <t>Призёр</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>14.02.2023</t>
+          <t>22.07.2021</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>13.02.2023</t>
+          <t>26.02.2023</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>13.02.2023</t>
+          <t>26.02.2023</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1221</t>
+          <t>ВСОШ по информатике</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Петрова Екатерина Андреевна</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>фывфыв</t>
+          <t>Жинжило Татьяна Кирилловна</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>География</t>
+          <t>Русский язык</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2б</t>
+          <t>9в</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Исскуство</t>
+          <t>Спорт</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Региональный</t>
+          <t>Школьный</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -585,17 +575,17 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>11.11.1111</t>
+          <t>12.12.2012</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>17.02.2023</t>
+          <t>26.02.2023</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>17.02.2023</t>
+          <t>26.02.2023</t>
         </is>
       </c>
     </row>

</xml_diff>